<commit_message>
Checking in updated MFHP SNOMED codes.
</commit_message>
<xml_diff>
--- a/documents/requirements/Data Set/code-systems-and-values-used-in-mfhp.xlsx
+++ b/documents/requirements/Data Set/code-systems-and-values-used-in-mfhp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="21580" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="27820" windowHeight="21700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,531 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="262">
+  <si>
+    <t>Rectal Cancer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rectal Cancer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>no current problems or disability</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Highlighted cells indicate changes to the original document.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>21611-9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diseases (some are subtypes of others)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>term displayed in app:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Races(some are subtypes of others)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gender</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>as of 2/21/2010</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code system and values used in MFHP v2.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>High Cholesterol</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>Dementia/Alzheimer's</t>
+  </si>
+  <si>
+    <t>Osteoporosis</t>
+  </si>
+  <si>
+    <t>Septicemia</t>
+  </si>
+  <si>
+    <t>Stroke/Brain Attack</t>
+  </si>
+  <si>
+    <t>Sudden Infant Death Syndrome</t>
+  </si>
+  <si>
+    <t>Type 1 Diabetes</t>
+  </si>
+  <si>
+    <t>Type 2 Diabetes</t>
+  </si>
+  <si>
+    <t>Gestational Diabetes</t>
+  </si>
+  <si>
+    <t>Diabetes Mellitus</t>
+  </si>
+  <si>
+    <t>Unknown Diabetes</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Attention Deficit Disorder-Hyperactivity</t>
+  </si>
+  <si>
+    <t>Autism</t>
+  </si>
+  <si>
+    <t>Bipolar Disorder</t>
+  </si>
+  <si>
+    <t>Dementia</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Eating Disorder</t>
+  </si>
+  <si>
+    <t>Obsessive Compulsive Disorder</t>
+  </si>
+  <si>
+    <t>Panic Disorder</t>
+  </si>
+  <si>
+    <t>Personality Disorder</t>
+  </si>
+  <si>
+    <t>Post Traumatic Stress Disorder</t>
+  </si>
+  <si>
+    <t>Schizophrenia</t>
+  </si>
+  <si>
+    <t>Social Phobia</t>
+  </si>
+  <si>
+    <t>Unspecified</t>
+  </si>
+  <si>
+    <t>Unknown Psychological Disorder</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>Chronic Bronchitis</t>
+  </si>
+  <si>
+    <t>Chronic Lower Respiratory Disease</t>
+  </si>
+  <si>
+    <t>COPD</t>
+  </si>
+  <si>
+    <t>Emphysema</t>
+  </si>
+  <si>
+    <t>Influenza/Pneumonia</t>
+  </si>
+  <si>
+    <t>Unknown Lung Disease</t>
+  </si>
+  <si>
+    <t>Cystic Kidney Disease</t>
+  </si>
+  <si>
+    <t>Diabetic Kidney Disease</t>
+  </si>
+  <si>
+    <t>Nephritis</t>
+  </si>
+  <si>
+    <t>Kidney Nephrosis</t>
+  </si>
+  <si>
+    <t>Nephrotic Syndrome</t>
+  </si>
+  <si>
+    <t>Unknown Kidney Disease</t>
+  </si>
+  <si>
+    <t>Kidney Disease Present from Birth</t>
+  </si>
+  <si>
+    <t>Other Kidney Disease</t>
+  </si>
+  <si>
+    <t>Bone Cancer</t>
+  </si>
+  <si>
+    <t>Breast Cancer</t>
+  </si>
+  <si>
+    <t>Colon Cancer</t>
+  </si>
+  <si>
+    <t>Esophageal Cancer</t>
+  </si>
+  <si>
+    <t>Gastric Cancer</t>
+  </si>
+  <si>
+    <t>Kidney Cancer</t>
+  </si>
+  <si>
+    <t>Leukemia</t>
+  </si>
+  <si>
+    <t>Lung Cancer</t>
+  </si>
+  <si>
+    <t>Muscle Cancer</t>
+  </si>
+  <si>
+    <t>Ovarian Cancer</t>
+  </si>
+  <si>
+    <t>Prostate Cancer</t>
+  </si>
+  <si>
+    <t>Skin Cancer</t>
+  </si>
+  <si>
+    <t>Thyroid Cancer</t>
+  </si>
+  <si>
+    <t>Uterine Cancer</t>
+  </si>
+  <si>
+    <t>Hereditary nonpolyposis colon cancer</t>
+  </si>
+  <si>
+    <t>Pancreatic cancer</t>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>29,729</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>childhood</t>
+  </si>
+  <si>
+    <t>2,9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Before age 20</t>
+  </si>
+  <si>
+    <t>10,19</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>At age 20-29</t>
+  </si>
+  <si>
+    <t>20,29</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>At age 30-39</t>
+  </si>
+  <si>
+    <t>30,39</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>At age 40-49</t>
+  </si>
+  <si>
+    <t>40,49</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>At age 50-59</t>
+  </si>
+  <si>
+    <t>50,59</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 and older</t>
+  </si>
+  <si>
+    <t>60</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age unknown</t>
+  </si>
+  <si>
+    <t>sis</t>
+  </si>
+  <si>
+    <t>Sister</t>
+  </si>
+  <si>
+    <t>bro</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>nsis</t>
+  </si>
+  <si>
+    <t>nbro</t>
+  </si>
+  <si>
+    <t>hsis</t>
+  </si>
+  <si>
+    <t>Half Sister</t>
+  </si>
+  <si>
+    <t>nephew</t>
+  </si>
+  <si>
+    <t>Nephew</t>
+  </si>
+  <si>
+    <t>niece</t>
+  </si>
+  <si>
+    <t>Niece</t>
+  </si>
+  <si>
+    <t>hbro</t>
+  </si>
+  <si>
+    <t>Half Brother</t>
+  </si>
+  <si>
+    <t>dau</t>
+  </si>
+  <si>
+    <t>Daughter</t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>grndau</t>
+  </si>
+  <si>
+    <t>Granddaughter</t>
+  </si>
+  <si>
+    <t>grnson</t>
+  </si>
+  <si>
+    <t>Grandson</t>
+  </si>
+  <si>
+    <t>grfth</t>
+  </si>
+  <si>
+    <t>Grandfather</t>
+  </si>
+  <si>
+    <t>mgrfth</t>
+  </si>
+  <si>
+    <t>Maternal Grandfather</t>
+  </si>
+  <si>
+    <t>pgrfth</t>
+  </si>
+  <si>
+    <t>not used in MFHP xml</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>values are low and high</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>values are low and high - no high range value for "60 and older"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2180-8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>the code system information is inaccurate in some places and will be changed in the future</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age Ranges:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relative codes(some of these would never show up in an xml file)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ethnicities(hispanic types are subtypes of hispanic or latino)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paternal Grandfather</t>
+  </si>
+  <si>
+    <t>grmth</t>
+  </si>
+  <si>
+    <t>Grandmother</t>
+  </si>
+  <si>
+    <t>mgrmth</t>
+  </si>
+  <si>
+    <t>Maternal Grandmother</t>
+  </si>
+  <si>
+    <t>pgrmth</t>
+  </si>
+  <si>
+    <t>Paternal Grandmother</t>
+  </si>
+  <si>
+    <t>aunt</t>
+  </si>
+  <si>
+    <t>Aunt</t>
+  </si>
+  <si>
+    <t>maunt</t>
+  </si>
+  <si>
+    <t>Maternal Aunt</t>
+  </si>
+  <si>
+    <t>paunt</t>
+  </si>
+  <si>
+    <t>Paternal Aunt</t>
+  </si>
+  <si>
+    <t>uncle</t>
+  </si>
+  <si>
+    <t>Uncle</t>
+  </si>
+  <si>
+    <t>muncle</t>
+  </si>
+  <si>
+    <t>Maternal Uncle</t>
+  </si>
+  <si>
+    <t>puncle</t>
+  </si>
+  <si>
+    <t>Paternal Uncle</t>
+  </si>
+  <si>
+    <t>cousn</t>
+  </si>
+  <si>
+    <t>Cousin</t>
+  </si>
+  <si>
+    <t>mcousn</t>
+  </si>
+  <si>
+    <t>Maternal Cousin</t>
+  </si>
+  <si>
+    <t>pcousn</t>
+  </si>
+  <si>
+    <t>Paternal Cousin</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>nmth</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Gastrointestinal Disorder</t>
+  </si>
+  <si>
+    <t>Unknown Gastrointestinal Disorder</t>
+  </si>
+  <si>
+    <t>Heart Disease</t>
+  </si>
+  <si>
+    <t>Heart Attack</t>
+  </si>
+  <si>
+    <t>Coronary Artery Disease</t>
+  </si>
+  <si>
+    <t>Angina</t>
+  </si>
+  <si>
+    <t>Unknown Heart Disease</t>
+  </si>
+  <si>
+    <t>Deep Vein Thrombosis (DVT)</t>
+  </si>
+  <si>
+    <t>Pulmonary Embolism</t>
+  </si>
+  <si>
+    <t>Clotting Disorder</t>
+  </si>
+  <si>
+    <t>Unknown Clotting Disorder</t>
+  </si>
+  <si>
+    <t>Unknown Disease</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Mental Disorder</t>
+  </si>
   <si>
     <t>nfth</t>
   </si>
@@ -37,39 +561,6 @@
   </si>
   <si>
     <t>LOINC</t>
-  </si>
-  <si>
-    <t>21611-9</t>
-  </si>
-  <si>
-    <t>21611-10</t>
-  </si>
-  <si>
-    <t>21611-11</t>
-  </si>
-  <si>
-    <t>21611-12</t>
-  </si>
-  <si>
-    <t>21611-13</t>
-  </si>
-  <si>
-    <t>21611-14</t>
-  </si>
-  <si>
-    <t>21611-15</t>
-  </si>
-  <si>
-    <t>21611-16</t>
-  </si>
-  <si>
-    <t>21611-17</t>
-  </si>
-  <si>
-    <t>21611-18</t>
-  </si>
-  <si>
-    <t>21611-19</t>
   </si>
   <si>
     <t>Estimated Age</t>
@@ -303,17 +794,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>original text: Parental consanguinity indicated</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Liver cancer</t>
   </si>
   <si>
     <t>Brain Cancer</t>
-  </si>
-  <si>
-    <t>Colorectal Cancer</t>
   </si>
   <si>
     <t>Familial multiple polyposis syndrome</t>
@@ -359,512 +843,6 @@
   </si>
   <si>
     <t>In infancy</t>
-  </si>
-  <si>
-    <t>29,729</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>childhood</t>
-  </si>
-  <si>
-    <t>2,9</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Before age 20</t>
-  </si>
-  <si>
-    <t>10,19</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>At age 20-29</t>
-  </si>
-  <si>
-    <t>20,29</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>At age 30-39</t>
-  </si>
-  <si>
-    <t>30,39</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>At age 40-49</t>
-  </si>
-  <si>
-    <t>40,49</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>At age 50-59</t>
-  </si>
-  <si>
-    <t>50,59</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>60 and older</t>
-  </si>
-  <si>
-    <t>60</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Age unknown</t>
-  </si>
-  <si>
-    <t>sis</t>
-  </si>
-  <si>
-    <t>Sister</t>
-  </si>
-  <si>
-    <t>bro</t>
-  </si>
-  <si>
-    <t>Brother</t>
-  </si>
-  <si>
-    <t>nsis</t>
-  </si>
-  <si>
-    <t>nbro</t>
-  </si>
-  <si>
-    <t>hsis</t>
-  </si>
-  <si>
-    <t>Half Sister</t>
-  </si>
-  <si>
-    <t>nephew</t>
-  </si>
-  <si>
-    <t>Nephew</t>
-  </si>
-  <si>
-    <t>niece</t>
-  </si>
-  <si>
-    <t>Niece</t>
-  </si>
-  <si>
-    <t>hbro</t>
-  </si>
-  <si>
-    <t>Half Brother</t>
-  </si>
-  <si>
-    <t>dau</t>
-  </si>
-  <si>
-    <t>Daughter</t>
-  </si>
-  <si>
-    <t>son</t>
-  </si>
-  <si>
-    <t>Son</t>
-  </si>
-  <si>
-    <t>grndau</t>
-  </si>
-  <si>
-    <t>Granddaughter</t>
-  </si>
-  <si>
-    <t>grnson</t>
-  </si>
-  <si>
-    <t>Grandson</t>
-  </si>
-  <si>
-    <t>grfth</t>
-  </si>
-  <si>
-    <t>Grandfather</t>
-  </si>
-  <si>
-    <t>mgrfth</t>
-  </si>
-  <si>
-    <t>Maternal Grandfather</t>
-  </si>
-  <si>
-    <t>pgrfth</t>
-  </si>
-  <si>
-    <t>not used in MFHP xml</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>values are low and high</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>values are low and high - no high range value for "60 and older"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2180-8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>the code system information is inaccurate in some places and will be changed in the future</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Age Ranges:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Relative codes(some of these would never show up in an xml file)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ethnicities(hispanic types are subtypes of hispanic or latino)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Paternal Grandfather</t>
-  </si>
-  <si>
-    <t>grmth</t>
-  </si>
-  <si>
-    <t>Grandmother</t>
-  </si>
-  <si>
-    <t>mgrmth</t>
-  </si>
-  <si>
-    <t>Maternal Grandmother</t>
-  </si>
-  <si>
-    <t>pgrmth</t>
-  </si>
-  <si>
-    <t>Paternal Grandmother</t>
-  </si>
-  <si>
-    <t>aunt</t>
-  </si>
-  <si>
-    <t>Aunt</t>
-  </si>
-  <si>
-    <t>maunt</t>
-  </si>
-  <si>
-    <t>Maternal Aunt</t>
-  </si>
-  <si>
-    <t>paunt</t>
-  </si>
-  <si>
-    <t>Paternal Aunt</t>
-  </si>
-  <si>
-    <t>uncle</t>
-  </si>
-  <si>
-    <t>Uncle</t>
-  </si>
-  <si>
-    <t>muncle</t>
-  </si>
-  <si>
-    <t>Maternal Uncle</t>
-  </si>
-  <si>
-    <t>puncle</t>
-  </si>
-  <si>
-    <t>Paternal Uncle</t>
-  </si>
-  <si>
-    <t>cousn</t>
-  </si>
-  <si>
-    <t>Cousin</t>
-  </si>
-  <si>
-    <t>mcousn</t>
-  </si>
-  <si>
-    <t>Maternal Cousin</t>
-  </si>
-  <si>
-    <t>pcousn</t>
-  </si>
-  <si>
-    <t>Paternal Cousin</t>
-  </si>
-  <si>
-    <t>self</t>
-  </si>
-  <si>
-    <t>Self</t>
-  </si>
-  <si>
-    <t>nmth</t>
-  </si>
-  <si>
-    <t>Mother</t>
-  </si>
-  <si>
-    <t>Gastrointestinal Disorder</t>
-  </si>
-  <si>
-    <t>Unknown Gastrointestinal Disorder</t>
-  </si>
-  <si>
-    <t>Heart Disease</t>
-  </si>
-  <si>
-    <t>Heart Attack</t>
-  </si>
-  <si>
-    <t>Coronary Artery Disease</t>
-  </si>
-  <si>
-    <t>Angina</t>
-  </si>
-  <si>
-    <t>Unknown Heart Disease</t>
-  </si>
-  <si>
-    <t>Deep Vein Thrombosis (DVT)</t>
-  </si>
-  <si>
-    <t>Pulmonary Embolism</t>
-  </si>
-  <si>
-    <t>Clotting Disorder</t>
-  </si>
-  <si>
-    <t>Unknown Clotting Disorder</t>
-  </si>
-  <si>
-    <t>Unknown Disease</t>
-  </si>
-  <si>
-    <t>Lung Disease (more options...)</t>
-  </si>
-  <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
-    <t>Mental Disorder</t>
-  </si>
-  <si>
-    <t>Diseases (some are subtypes of others)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>term displayed in app:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Races(some are subtypes of others)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gender</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>as of 2/21/2010</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code system and values used in MFHP v2.3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>High Cholesterol</t>
-  </si>
-  <si>
-    <t>Hypertension</t>
-  </si>
-  <si>
-    <t>Lung Disease</t>
-  </si>
-  <si>
-    <t>Dementia/Alzheimer's</t>
-  </si>
-  <si>
-    <t>Osteoporosis</t>
-  </si>
-  <si>
-    <t>Septicemia</t>
-  </si>
-  <si>
-    <t>Stroke/Brain Attack</t>
-  </si>
-  <si>
-    <t>Sudden Infant Death Syndrome</t>
-  </si>
-  <si>
-    <t>Type 1 Diabetes</t>
-  </si>
-  <si>
-    <t>Type 2 Diabetes</t>
-  </si>
-  <si>
-    <t>Gestational Diabetes</t>
-  </si>
-  <si>
-    <t>Diabetes Mellitus</t>
-  </si>
-  <si>
-    <t>Unknown Diabetes</t>
-  </si>
-  <si>
-    <t>Anxiety</t>
-  </si>
-  <si>
-    <t>Attention Deficit Disorder-Hyperactivity</t>
-  </si>
-  <si>
-    <t>Autism</t>
-  </si>
-  <si>
-    <t>Bipolar Disorder</t>
-  </si>
-  <si>
-    <t>Dementia</t>
-  </si>
-  <si>
-    <t>Depression</t>
-  </si>
-  <si>
-    <t>Eating Disorder</t>
-  </si>
-  <si>
-    <t>Obsessive Compulsive Disorder</t>
-  </si>
-  <si>
-    <t>Panic Disorder</t>
-  </si>
-  <si>
-    <t>Personality Disorder</t>
-  </si>
-  <si>
-    <t>Post Traumatic Stress Disorder</t>
-  </si>
-  <si>
-    <t>Schizophrenia</t>
-  </si>
-  <si>
-    <t>Social Phobia</t>
-  </si>
-  <si>
-    <t>Unspecified</t>
-  </si>
-  <si>
-    <t>Unknown Psychological Disorder</t>
-  </si>
-  <si>
-    <t>Asthma</t>
-  </si>
-  <si>
-    <t>Chronic Bronchitis</t>
-  </si>
-  <si>
-    <t>Chronic Lower Respiratory Disease</t>
-  </si>
-  <si>
-    <t>COPD</t>
-  </si>
-  <si>
-    <t>Emphysema</t>
-  </si>
-  <si>
-    <t>Influenza/Pneumonia</t>
-  </si>
-  <si>
-    <t>Unknown Lung Disease</t>
-  </si>
-  <si>
-    <t>Cystic Kidney Disease</t>
-  </si>
-  <si>
-    <t>Diabetic Kidney Disease</t>
-  </si>
-  <si>
-    <t>Nephritis</t>
-  </si>
-  <si>
-    <t>Kidney Nephrosis</t>
-  </si>
-  <si>
-    <t>Nephrotic Syndrome</t>
-  </si>
-  <si>
-    <t>Unknown Kidney Disease</t>
-  </si>
-  <si>
-    <t>Kidney Disease Present from Birth</t>
-  </si>
-  <si>
-    <t>Other Kidney Disease</t>
-  </si>
-  <si>
-    <t>Bone Cancer</t>
-  </si>
-  <si>
-    <t>Breast Cancer</t>
-  </si>
-  <si>
-    <t>Colon Cancer</t>
-  </si>
-  <si>
-    <t>Esophageal Cancer</t>
-  </si>
-  <si>
-    <t>Gastric Cancer</t>
-  </si>
-  <si>
-    <t>Kidney Cancer</t>
-  </si>
-  <si>
-    <t>Leukemia</t>
-  </si>
-  <si>
-    <t>Lung Cancer</t>
-  </si>
-  <si>
-    <t>Muscle Cancer</t>
-  </si>
-  <si>
-    <t>Ovarian Cancer</t>
-  </si>
-  <si>
-    <t>Prostate Cancer</t>
-  </si>
-  <si>
-    <t>Skin Cancer</t>
-  </si>
-  <si>
-    <t>Thyroid Cancer</t>
-  </si>
-  <si>
-    <t>Uterine Cancer</t>
-  </si>
-  <si>
-    <t>Hereditary nonpolyposis colon cancer</t>
-  </si>
-  <si>
-    <t>Pancreatic cancer</t>
   </si>
 </sst>
 </file>
@@ -903,7 +881,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -913,6 +891,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1087,7 +1077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1162,6 +1152,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,59 +1494,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="32"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="2.28515625" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>211</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="48" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>81</v>
+        <v>235</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>82</v>
+        <v>236</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>83</v>
+        <v>237</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>103</v>
+        <v>255</v>
       </c>
       <c r="F4" s="48" t="s">
-        <v>90</v>
+        <v>244</v>
       </c>
       <c r="G4" s="48"/>
       <c r="H4" s="51" t="s">
-        <v>91</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="13" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="15"/>
@@ -1556,258 +1561,258 @@
     <row r="6" spans="1:8">
       <c r="A6" s="7"/>
       <c r="B6" s="34" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>105</v>
+        <v>257</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>106</v>
+        <v>258</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="4"/>
-      <c r="B7" s="35" t="s">
-        <v>7</v>
+      <c r="B7" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>108</v>
+        <v>260</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>106</v>
+        <v>258</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>107</v>
+        <v>259</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="4"/>
-      <c r="B8" s="35" t="s">
-        <v>8</v>
+      <c r="B8" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>106</v>
+        <v>258</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>109</v>
+        <v>261</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4"/>
-      <c r="B9" s="35" t="s">
-        <v>9</v>
+      <c r="B9" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4"/>
-      <c r="B10" s="35" t="s">
-        <v>10</v>
+      <c r="B10" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4"/>
-      <c r="B11" s="35" t="s">
-        <v>11</v>
+      <c r="B11" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4"/>
-      <c r="B12" s="35" t="s">
-        <v>12</v>
+      <c r="B12" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4"/>
-      <c r="B13" s="35" t="s">
-        <v>13</v>
+      <c r="B13" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4"/>
-      <c r="B14" s="35" t="s">
-        <v>14</v>
+      <c r="B14" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="26">
       <c r="A15" s="4"/>
-      <c r="B15" s="35" t="s">
-        <v>15</v>
+      <c r="B15" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="10"/>
-      <c r="B16" s="36" t="s">
-        <v>16</v>
+      <c r="B16" s="34" t="s">
+        <v>4</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="H16" s="12"/>
     </row>
@@ -1823,7 +1828,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="21" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="23"/>
@@ -1836,49 +1841,49 @@
     <row r="19" spans="1:8">
       <c r="A19" s="7"/>
       <c r="B19" s="34" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="9" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="35" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="6" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="4"/>
       <c r="B21" s="35" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="4"/>
@@ -1888,13 +1893,13 @@
     <row r="22" spans="1:8">
       <c r="A22" s="4"/>
       <c r="B22" s="35" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="4"/>
@@ -1904,13 +1909,13 @@
     <row r="23" spans="1:8">
       <c r="A23" s="4"/>
       <c r="B23" s="35" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="4"/>
@@ -1920,13 +1925,13 @@
     <row r="24" spans="1:8">
       <c r="A24" s="4"/>
       <c r="B24" s="35" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="4"/>
@@ -1936,13 +1941,13 @@
     <row r="25" spans="1:8">
       <c r="A25" s="4"/>
       <c r="B25" s="35" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="4"/>
@@ -1952,13 +1957,13 @@
     <row r="26" spans="1:8">
       <c r="A26" s="4"/>
       <c r="B26" s="35" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="4"/>
@@ -1968,13 +1973,13 @@
     <row r="27" spans="1:8">
       <c r="A27" s="4"/>
       <c r="B27" s="35" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="4"/>
@@ -1984,13 +1989,13 @@
     <row r="28" spans="1:8">
       <c r="A28" s="4"/>
       <c r="B28" s="35" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="4"/>
@@ -2000,13 +2005,13 @@
     <row r="29" spans="1:8">
       <c r="A29" s="4"/>
       <c r="B29" s="35" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="4"/>
@@ -2016,13 +2021,13 @@
     <row r="30" spans="1:8">
       <c r="A30" s="4"/>
       <c r="B30" s="35" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="4"/>
@@ -2032,31 +2037,31 @@
     <row r="31" spans="1:8">
       <c r="A31" s="4"/>
       <c r="B31" s="35" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="6" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4"/>
       <c r="B32" s="35" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="4"/>
@@ -2066,13 +2071,13 @@
     <row r="33" spans="1:8">
       <c r="A33" s="4"/>
       <c r="B33" s="35" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
@@ -2082,31 +2087,31 @@
     <row r="34" spans="1:8">
       <c r="A34" s="4"/>
       <c r="B34" s="35" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="6" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="4"/>
       <c r="B35" s="35" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="4"/>
@@ -2116,13 +2121,13 @@
     <row r="36" spans="1:8">
       <c r="A36" s="4"/>
       <c r="B36" s="35" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="4"/>
@@ -2132,31 +2137,31 @@
     <row r="37" spans="1:8">
       <c r="A37" s="4"/>
       <c r="B37" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D37" s="4" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="6" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="4"/>
       <c r="B38" s="35" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="4"/>
@@ -2166,13 +2171,13 @@
     <row r="39" spans="1:8">
       <c r="A39" s="4"/>
       <c r="B39" s="35" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="4"/>
@@ -2182,31 +2187,31 @@
     <row r="40" spans="1:8">
       <c r="A40" s="4"/>
       <c r="B40" s="35" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="6" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="4"/>
       <c r="B41" s="35" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="4"/>
@@ -2216,13 +2221,13 @@
     <row r="42" spans="1:8">
       <c r="A42" s="4"/>
       <c r="B42" s="35" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="4"/>
@@ -2232,31 +2237,31 @@
     <row r="43" spans="1:8">
       <c r="A43" s="4"/>
       <c r="B43" s="35" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="6" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4"/>
       <c r="B44" s="35" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="4"/>
@@ -2266,13 +2271,13 @@
     <row r="45" spans="1:8">
       <c r="A45" s="4"/>
       <c r="B45" s="35" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="4"/>
@@ -2282,13 +2287,13 @@
     <row r="46" spans="1:8">
       <c r="A46" s="4"/>
       <c r="B46" s="35" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="4"/>
@@ -2298,13 +2303,13 @@
     <row r="47" spans="1:8">
       <c r="A47" s="4"/>
       <c r="B47" s="35" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="4"/>
@@ -2314,13 +2319,13 @@
     <row r="48" spans="1:8">
       <c r="A48" s="4"/>
       <c r="B48" s="35" t="s">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="4"/>
@@ -2330,13 +2335,13 @@
     <row r="49" spans="1:8">
       <c r="A49" s="10"/>
       <c r="B49" s="36" t="s">
-        <v>2</v>
+        <v>167</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>3</v>
+        <v>168</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="10"/>
@@ -2355,7 +2360,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="21" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="B51" s="40"/>
       <c r="C51" s="30"/>
@@ -2368,31 +2373,31 @@
     <row r="52" spans="1:8" ht="39">
       <c r="A52" s="7"/>
       <c r="B52" s="34" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="9" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="4"/>
       <c r="B53" s="35" t="s">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="4"/>
@@ -2402,13 +2407,13 @@
     <row r="54" spans="1:8">
       <c r="A54" s="4"/>
       <c r="B54" s="35" t="s">
-        <v>19</v>
+        <v>173</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="4"/>
@@ -2418,13 +2423,13 @@
     <row r="55" spans="1:8">
       <c r="A55" s="4"/>
       <c r="B55" s="35" t="s">
-        <v>20</v>
+        <v>174</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="4"/>
@@ -2434,13 +2439,13 @@
     <row r="56" spans="1:8">
       <c r="A56" s="4"/>
       <c r="B56" s="35" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="4"/>
@@ -2450,13 +2455,13 @@
     <row r="57" spans="1:8">
       <c r="A57" s="4"/>
       <c r="B57" s="35" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="4"/>
@@ -2466,13 +2471,13 @@
     <row r="58" spans="1:8">
       <c r="A58" s="4"/>
       <c r="B58" s="35" t="s">
-        <v>23</v>
+        <v>177</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="4"/>
@@ -2485,10 +2490,10 @@
         <v>1000000</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="4"/>
@@ -2498,13 +2503,13 @@
     <row r="60" spans="1:8">
       <c r="A60" s="4"/>
       <c r="B60" s="35" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="4"/>
@@ -2514,13 +2519,13 @@
     <row r="61" spans="1:8">
       <c r="A61" s="10"/>
       <c r="B61" s="36" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="10"/>
@@ -2539,7 +2544,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="21" t="s">
-        <v>208</v>
+        <v>7</v>
       </c>
       <c r="B63" s="40"/>
       <c r="C63" s="30"/>
@@ -2552,13 +2557,13 @@
     <row r="64" spans="1:8">
       <c r="A64" s="7"/>
       <c r="B64" s="34" t="s">
-        <v>44</v>
+        <v>198</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>45</v>
+        <v>199</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
@@ -2568,31 +2573,31 @@
     <row r="65" spans="1:8" ht="39">
       <c r="A65" s="4"/>
       <c r="B65" s="35" t="s">
-        <v>46</v>
+        <v>200</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="6" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="4"/>
       <c r="B66" s="35" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="4"/>
@@ -2602,13 +2607,13 @@
     <row r="67" spans="1:8">
       <c r="A67" s="4"/>
       <c r="B67" s="35" t="s">
-        <v>50</v>
+        <v>204</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>51</v>
+        <v>205</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="4"/>
@@ -2618,13 +2623,13 @@
     <row r="68" spans="1:8">
       <c r="A68" s="4"/>
       <c r="B68" s="35" t="s">
-        <v>52</v>
+        <v>206</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>53</v>
+        <v>207</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="4"/>
@@ -2634,13 +2639,13 @@
     <row r="69" spans="1:8">
       <c r="A69" s="4"/>
       <c r="B69" s="35" t="s">
-        <v>54</v>
+        <v>208</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>55</v>
+        <v>209</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="4"/>
@@ -2650,13 +2655,13 @@
     <row r="70" spans="1:8">
       <c r="A70" s="4"/>
       <c r="B70" s="35" t="s">
-        <v>56</v>
+        <v>210</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>57</v>
+        <v>211</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="4"/>
@@ -2666,13 +2671,13 @@
     <row r="71" spans="1:8">
       <c r="A71" s="4"/>
       <c r="B71" s="35" t="s">
-        <v>58</v>
+        <v>212</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>59</v>
+        <v>213</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="4"/>
@@ -2682,13 +2687,13 @@
     <row r="72" spans="1:8">
       <c r="A72" s="4"/>
       <c r="B72" s="35" t="s">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="4"/>
@@ -2698,13 +2703,13 @@
     <row r="73" spans="1:8">
       <c r="A73" s="4"/>
       <c r="B73" s="35" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>63</v>
+        <v>217</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="4"/>
@@ -2714,13 +2719,13 @@
     <row r="74" spans="1:8">
       <c r="A74" s="4"/>
       <c r="B74" s="35" t="s">
-        <v>64</v>
+        <v>218</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="4"/>
@@ -2730,13 +2735,13 @@
     <row r="75" spans="1:8">
       <c r="A75" s="4"/>
       <c r="B75" s="35" t="s">
-        <v>66</v>
+        <v>220</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>67</v>
+        <v>221</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>68</v>
+        <v>222</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="4"/>
@@ -2746,13 +2751,13 @@
     <row r="76" spans="1:8">
       <c r="A76" s="4"/>
       <c r="B76" s="35" t="s">
-        <v>69</v>
+        <v>223</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>70</v>
+        <v>224</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="4"/>
@@ -2762,13 +2767,13 @@
     <row r="77" spans="1:8">
       <c r="A77" s="4"/>
       <c r="B77" s="35" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="4"/>
@@ -2778,13 +2783,13 @@
     <row r="78" spans="1:8">
       <c r="A78" s="4"/>
       <c r="B78" s="35" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>74</v>
+        <v>228</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="4"/>
@@ -2794,13 +2799,13 @@
     <row r="79" spans="1:8">
       <c r="A79" s="4"/>
       <c r="B79" s="35" t="s">
-        <v>75</v>
+        <v>229</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>76</v>
+        <v>230</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="4"/>
@@ -2810,13 +2815,13 @@
     <row r="80" spans="1:8">
       <c r="A80" s="4"/>
       <c r="B80" s="35" t="s">
-        <v>77</v>
+        <v>231</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>78</v>
+        <v>232</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="4"/>
@@ -2826,13 +2831,13 @@
     <row r="81" spans="1:8" ht="26">
       <c r="A81" s="10"/>
       <c r="B81" s="36" t="s">
-        <v>79</v>
+        <v>233</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>80</v>
+        <v>234</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="10"/>
@@ -2851,7 +2856,7 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="21" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="B83" s="40"/>
       <c r="C83" s="30"/>
@@ -2864,13 +2869,13 @@
     <row r="84" spans="1:8">
       <c r="A84" s="7"/>
       <c r="B84" s="34" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>27</v>
+        <v>181</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="7"/>
@@ -2880,13 +2885,13 @@
     <row r="85" spans="1:8">
       <c r="A85" s="10"/>
       <c r="B85" s="36" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>29</v>
+        <v>183</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="10"/>
@@ -2905,7 +2910,7 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="47" t="s">
-        <v>88</v>
+        <v>242</v>
       </c>
       <c r="B87" s="40"/>
       <c r="C87" s="30"/>
@@ -2921,10 +2926,10 @@
         <v>313415001</v>
       </c>
       <c r="C88" s="34" t="s">
-        <v>84</v>
+        <v>238</v>
       </c>
       <c r="D88" s="34" t="s">
-        <v>85</v>
+        <v>239</v>
       </c>
       <c r="E88" s="43"/>
       <c r="F88" s="44"/>
@@ -2937,10 +2942,10 @@
         <v>313416000</v>
       </c>
       <c r="C89" s="34" t="s">
-        <v>84</v>
+        <v>238</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>86</v>
+        <v>240</v>
       </c>
       <c r="E89" s="26"/>
       <c r="F89" s="27"/>
@@ -2953,17 +2958,17 @@
         <v>160496001</v>
       </c>
       <c r="C90" s="34" t="s">
-        <v>84</v>
+        <v>238</v>
       </c>
       <c r="D90" s="35" t="s">
-        <v>87</v>
+        <v>241</v>
       </c>
       <c r="E90" s="26"/>
       <c r="F90" s="27"/>
       <c r="G90" s="27"/>
       <c r="H90" s="28"/>
     </row>
-    <row r="91" spans="1:8" ht="26">
+    <row r="91" spans="1:8">
       <c r="A91" s="25"/>
       <c r="B91" s="39"/>
       <c r="C91" s="46"/>
@@ -2972,7 +2977,7 @@
       <c r="F91" s="27"/>
       <c r="G91" s="27"/>
       <c r="H91" s="28" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2987,7 +2992,7 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="21" t="s">
-        <v>206</v>
+        <v>5</v>
       </c>
       <c r="B93" s="40"/>
       <c r="C93" s="30"/>
@@ -2996,7 +3001,7 @@
       <c r="F93" s="30"/>
       <c r="G93" s="30"/>
       <c r="H93" s="24" t="s">
-        <v>207</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3005,16 +3010,16 @@
         <v>55822004</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>212</v>
+        <v>11</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4" t="s">
-        <v>212</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -3023,1094 +3028,1090 @@
         <v>38341003</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>213</v>
+        <v>12</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4" t="s">
-        <v>213</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="4"/>
       <c r="B96" s="41">
-        <v>19829001</v>
+        <v>26929004</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>214</v>
+        <v>13</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="4"/>
       <c r="B97" s="41">
-        <v>26929004</v>
+        <v>64859006</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="4"/>
-      <c r="B98" s="41">
-        <v>64859006</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E98" s="5"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4" t="s">
-        <v>216</v>
+      <c r="B98" s="57">
+        <v>10001005</v>
+      </c>
+      <c r="C98" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D98" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" s="58"/>
+      <c r="F98" s="54"/>
+      <c r="G98" s="54"/>
+      <c r="H98" s="54" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="4"/>
-      <c r="B99" s="41">
-        <v>105592009</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="E99" s="5"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4" t="s">
-        <v>217</v>
+      <c r="B99" s="57">
+        <v>422504002</v>
+      </c>
+      <c r="C99" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D99" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E99" s="58"/>
+      <c r="F99" s="54"/>
+      <c r="G99" s="54"/>
+      <c r="H99" s="54" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" s="4"/>
       <c r="B100" s="41">
-        <v>116288000</v>
+        <v>51178009</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4" t="s">
-        <v>218</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="4"/>
       <c r="B101" s="41">
-        <v>51178009</v>
+        <v>46635009</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>219</v>
+        <v>18</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4" t="s">
-        <v>219</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" s="4"/>
       <c r="B102" s="41">
-        <v>46635009</v>
+        <v>44054006</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>220</v>
+        <v>19</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4" t="s">
-        <v>220</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" s="4"/>
       <c r="B103" s="41">
-        <v>44054006</v>
+        <v>11687002</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>221</v>
+        <v>20</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4" t="s">
-        <v>221</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" s="4"/>
       <c r="B104" s="41">
-        <v>11687002</v>
+        <v>73211009</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>222</v>
+        <v>21</v>
       </c>
       <c r="E104" s="5"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4" t="s">
-        <v>222</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="4"/>
-      <c r="B105" s="41">
-        <v>73211009</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="E105" s="5"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4" t="s">
-        <v>204</v>
+      <c r="B105" s="61"/>
+      <c r="C105" s="59"/>
+      <c r="D105" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" s="62"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="59"/>
+      <c r="H105" s="59" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" s="4"/>
-      <c r="B106" s="41"/>
-      <c r="C106" s="4"/>
+      <c r="B106" s="41">
+        <v>48694002</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D106" s="4" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" s="4"/>
       <c r="B107" s="41">
-        <v>197480006</v>
+        <v>406506008</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>225</v>
+        <v>24</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4" t="s">
-        <v>225</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" s="4"/>
       <c r="B108" s="41">
-        <v>406506008</v>
+        <v>408856003</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>226</v>
+        <v>25</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4" t="s">
-        <v>226</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" s="4"/>
       <c r="B109" s="41">
-        <v>408856003</v>
+        <v>13746004</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>227</v>
+        <v>26</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4" t="s">
-        <v>227</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110" s="4"/>
       <c r="B110" s="41">
-        <v>13746004</v>
+        <v>52448006</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" s="4"/>
       <c r="B111" s="41">
-        <v>52448006</v>
+        <v>35489007</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>229</v>
+        <v>28</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4" t="s">
-        <v>229</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="4"/>
       <c r="B112" s="41">
-        <v>35489007</v>
+        <v>72366004</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>230</v>
+        <v>29</v>
       </c>
       <c r="E112" s="5"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4" t="s">
-        <v>230</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" s="4"/>
       <c r="B113" s="41">
-        <v>72366004</v>
+        <v>191736004</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>231</v>
+        <v>30</v>
       </c>
       <c r="E113" s="5"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4" t="s">
-        <v>231</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" s="4"/>
       <c r="B114" s="41">
-        <v>191736004</v>
+        <v>371631005</v>
       </c>
       <c r="C114" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D114" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>232</v>
       </c>
       <c r="E114" s="5"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4" t="s">
-        <v>232</v>
+        <v>31</v>
       </c>
     </row>
     <row r="115" spans="1:8">
       <c r="A115" s="4"/>
       <c r="B115" s="41">
-        <v>371631005</v>
+        <v>33449004</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" s="4"/>
       <c r="B116" s="41">
-        <v>33449004</v>
+        <v>47505003</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="E116" s="5"/>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="1:8">
       <c r="A117" s="4"/>
       <c r="B117" s="41">
-        <v>47505003</v>
+        <v>58214004</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
       <c r="E117" s="5"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" s="4"/>
       <c r="B118" s="41">
-        <v>58214004</v>
+        <v>25501002</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
     </row>
     <row r="119" spans="1:8">
       <c r="A119" s="4"/>
       <c r="B119" s="41">
-        <v>25501002</v>
+        <v>74732009</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>237</v>
+        <v>36</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4" t="s">
-        <v>237</v>
+        <v>164</v>
       </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" s="4"/>
-      <c r="B120" s="41">
-        <v>74732009</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B120" s="41"/>
+      <c r="C120" s="4"/>
       <c r="D120" s="4" t="s">
-        <v>238</v>
+        <v>37</v>
       </c>
       <c r="E120" s="5"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4" t="s">
-        <v>205</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:8">
       <c r="A121" s="4"/>
-      <c r="B121" s="41"/>
-      <c r="C121" s="4"/>
+      <c r="B121" s="41">
+        <v>195967001</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D121" s="4" t="s">
-        <v>239</v>
+        <v>38</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4" t="s">
-        <v>239</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122" spans="1:8">
       <c r="A122" s="4"/>
       <c r="B122" s="41">
-        <v>195967001</v>
+        <v>63480004</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="E122" s="5"/>
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4" t="s">
-        <v>240</v>
+        <v>39</v>
       </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" s="4"/>
       <c r="B123" s="41">
-        <v>63480004</v>
+        <v>196229000</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>241</v>
+        <v>40</v>
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="4"/>
       <c r="G123" s="4"/>
       <c r="H123" s="4" t="s">
-        <v>241</v>
+        <v>40</v>
       </c>
     </row>
     <row r="124" spans="1:8">
       <c r="A124" s="4"/>
       <c r="B124" s="41">
-        <v>196229000</v>
+        <v>13645005</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="4"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" s="4"/>
       <c r="B125" s="41">
-        <v>13645005</v>
+        <v>87433001</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>243</v>
+        <v>42</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4" t="s">
-        <v>243</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="1:8">
       <c r="A126" s="4"/>
       <c r="B126" s="41">
-        <v>87433001</v>
+        <v>195878008</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>244</v>
+        <v>43</v>
       </c>
       <c r="E126" s="5"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4" t="s">
-        <v>244</v>
+        <v>43</v>
       </c>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" s="4"/>
-      <c r="B127" s="41">
-        <v>195878008</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B127" s="41"/>
+      <c r="C127" s="4"/>
       <c r="D127" s="4" t="s">
-        <v>245</v>
+        <v>44</v>
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4" t="s">
-        <v>245</v>
+        <v>44</v>
       </c>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" s="4"/>
-      <c r="B128" s="41"/>
-      <c r="C128" s="4"/>
+      <c r="B128" s="41">
+        <v>236439005</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D128" s="4" t="s">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="E128" s="5"/>
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
       <c r="H128" s="4" t="s">
-        <v>246</v>
+        <v>45</v>
       </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="4"/>
       <c r="B129" s="41">
-        <v>236439005</v>
+        <v>127013003</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>247</v>
+        <v>46</v>
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="4"/>
       <c r="G129" s="4"/>
       <c r="H129" s="4" t="s">
-        <v>247</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" s="4"/>
       <c r="B130" s="41">
-        <v>127013003</v>
+        <v>52845002</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>248</v>
+        <v>47</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="4"/>
       <c r="G130" s="4"/>
       <c r="H130" s="4" t="s">
-        <v>248</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:8">
       <c r="A131" s="4"/>
       <c r="B131" s="41">
-        <v>52845002</v>
+        <v>90708001</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>249</v>
+        <v>48</v>
       </c>
       <c r="E131" s="5"/>
       <c r="F131" s="4"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4" t="s">
-        <v>249</v>
+        <v>48</v>
       </c>
     </row>
     <row r="132" spans="1:8">
       <c r="A132" s="4"/>
       <c r="B132" s="41">
-        <v>90708001</v>
+        <v>52254009</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="E132" s="5"/>
       <c r="F132" s="4"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" s="4"/>
-      <c r="B133" s="41">
-        <v>52254009</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B133" s="41"/>
+      <c r="C133" s="4"/>
       <c r="D133" s="4" t="s">
-        <v>251</v>
+        <v>50</v>
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="4"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4" t="s">
-        <v>251</v>
+        <v>50</v>
       </c>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" s="4"/>
-      <c r="B134" s="41"/>
-      <c r="C134" s="4"/>
+      <c r="B134" s="41">
+        <v>82525005</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D134" s="4" t="s">
-        <v>252</v>
+        <v>51</v>
       </c>
       <c r="E134" s="5"/>
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4" t="s">
-        <v>252</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="4"/>
-      <c r="B135" s="41">
-        <v>82525005</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B135" s="41"/>
+      <c r="C135" s="4"/>
       <c r="D135" s="4" t="s">
-        <v>253</v>
+        <v>52</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="4"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4" t="s">
-        <v>253</v>
+        <v>52</v>
       </c>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" s="4"/>
-      <c r="B136" s="41"/>
-      <c r="C136" s="4"/>
+      <c r="B136" s="41">
+        <v>269466003</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D136" s="4" t="s">
-        <v>254</v>
+        <v>53</v>
       </c>
       <c r="E136" s="5"/>
       <c r="F136" s="4"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4" t="s">
-        <v>254</v>
+        <v>53</v>
       </c>
     </row>
     <row r="137" spans="1:8">
       <c r="A137" s="4"/>
       <c r="B137" s="41">
-        <v>269466003</v>
+        <v>254837009</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>255</v>
+        <v>54</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="4"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4" t="s">
-        <v>255</v>
+        <v>54</v>
       </c>
     </row>
     <row r="138" spans="1:8">
       <c r="A138" s="4"/>
       <c r="B138" s="41">
-        <v>254837009</v>
+        <v>363406005</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>256</v>
+        <v>55</v>
       </c>
       <c r="E138" s="5"/>
       <c r="F138" s="4"/>
       <c r="G138" s="4"/>
       <c r="H138" s="4" t="s">
-        <v>256</v>
+        <v>55</v>
       </c>
     </row>
     <row r="139" spans="1:8">
       <c r="A139" s="4"/>
       <c r="B139" s="41">
-        <v>363406005</v>
+        <v>363402007</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>257</v>
+        <v>56</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="4"/>
       <c r="G139" s="4"/>
       <c r="H139" s="4" t="s">
-        <v>257</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:8">
       <c r="A140" s="4"/>
       <c r="B140" s="41">
-        <v>363402007</v>
+        <v>363349007</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>258</v>
+        <v>57</v>
       </c>
       <c r="E140" s="5"/>
       <c r="F140" s="4"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4" t="s">
-        <v>258</v>
+        <v>57</v>
       </c>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" s="4"/>
       <c r="B141" s="41">
-        <v>363349007</v>
+        <v>363518003</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>259</v>
+        <v>58</v>
       </c>
       <c r="E141" s="5"/>
       <c r="F141" s="4"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4" t="s">
-        <v>259</v>
+        <v>58</v>
       </c>
     </row>
     <row r="142" spans="1:8">
       <c r="A142" s="4"/>
       <c r="B142" s="41">
-        <v>363518003</v>
+        <v>93143009</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>260</v>
+        <v>59</v>
       </c>
       <c r="E142" s="5"/>
       <c r="F142" s="4"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4" t="s">
-        <v>260</v>
+        <v>59</v>
       </c>
     </row>
     <row r="143" spans="1:8">
       <c r="A143" s="4"/>
       <c r="B143" s="41">
-        <v>93143009</v>
+        <v>93880001</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>261</v>
+        <v>60</v>
       </c>
       <c r="E143" s="5"/>
       <c r="F143" s="4"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4" t="s">
-        <v>261</v>
+        <v>60</v>
       </c>
     </row>
     <row r="144" spans="1:8">
       <c r="A144" s="4"/>
       <c r="B144" s="41">
-        <v>363358000</v>
+        <v>363495004</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>262</v>
+        <v>61</v>
       </c>
       <c r="E144" s="5"/>
       <c r="F144" s="4"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4" t="s">
-        <v>262</v>
+        <v>61</v>
       </c>
     </row>
     <row r="145" spans="1:8">
       <c r="A145" s="4"/>
       <c r="B145" s="41">
-        <v>363495004</v>
+        <v>363443007</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>263</v>
+        <v>62</v>
       </c>
       <c r="E145" s="5"/>
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
       <c r="H145" s="4" t="s">
-        <v>263</v>
+        <v>62</v>
       </c>
     </row>
     <row r="146" spans="1:8">
       <c r="A146" s="4"/>
       <c r="B146" s="41">
-        <v>363443007</v>
+        <v>399068003</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>264</v>
+        <v>63</v>
       </c>
       <c r="E146" s="5"/>
       <c r="F146" s="4"/>
       <c r="G146" s="4"/>
       <c r="H146" s="4" t="s">
-        <v>264</v>
+        <v>63</v>
       </c>
     </row>
     <row r="147" spans="1:8">
       <c r="A147" s="4"/>
       <c r="B147" s="41">
-        <v>399068003</v>
+        <v>372130007</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>265</v>
+        <v>64</v>
       </c>
       <c r="E147" s="5"/>
       <c r="F147" s="4"/>
       <c r="G147" s="4"/>
       <c r="H147" s="4" t="s">
-        <v>265</v>
+        <v>64</v>
       </c>
     </row>
     <row r="148" spans="1:8">
       <c r="A148" s="4"/>
       <c r="B148" s="41">
-        <v>372130007</v>
+        <v>363478007</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>266</v>
+        <v>65</v>
       </c>
       <c r="E148" s="5"/>
       <c r="F148" s="4"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4" t="s">
-        <v>266</v>
+        <v>65</v>
       </c>
     </row>
     <row r="149" spans="1:8">
       <c r="A149" s="4"/>
       <c r="B149" s="41">
-        <v>363478007</v>
+        <v>371973000</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
       <c r="E149" s="5"/>
       <c r="F149" s="4"/>
       <c r="G149" s="4"/>
       <c r="H149" s="4" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
     </row>
     <row r="150" spans="1:8">
       <c r="A150" s="4"/>
       <c r="B150" s="41">
-        <v>371973000</v>
+        <v>315058005</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>268</v>
+        <v>67</v>
       </c>
       <c r="E150" s="5"/>
       <c r="F150" s="4"/>
       <c r="G150" s="4"/>
       <c r="H150" s="4" t="s">
-        <v>268</v>
+        <v>67</v>
       </c>
     </row>
     <row r="151" spans="1:8">
       <c r="A151" s="4"/>
       <c r="B151" s="41">
-        <v>315058005</v>
+        <v>363418001</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>269</v>
+        <v>68</v>
       </c>
       <c r="E151" s="5"/>
       <c r="F151" s="4"/>
       <c r="G151" s="4"/>
       <c r="H151" s="4" t="s">
-        <v>269</v>
+        <v>68</v>
       </c>
     </row>
     <row r="152" spans="1:8">
       <c r="A152" s="4"/>
       <c r="B152" s="41">
-        <v>363418001</v>
+        <v>93870000</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="E152" s="5"/>
       <c r="F152" s="4"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" s="4"/>
-      <c r="B153" s="41">
-        <v>93870000</v>
-      </c>
-      <c r="C153" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E153" s="5"/>
-      <c r="F153" s="4"/>
-      <c r="G153" s="4"/>
-      <c r="H153" s="4" t="s">
-        <v>93</v>
+      <c r="B153" s="57">
+        <v>126952004</v>
+      </c>
+      <c r="C153" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D153" s="54" t="s">
+        <v>247</v>
+      </c>
+      <c r="E153" s="58"/>
+      <c r="F153" s="54"/>
+      <c r="G153" s="54"/>
+      <c r="H153" s="54" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="154" spans="1:8">
       <c r="A154" s="4"/>
-      <c r="B154" s="41">
-        <v>1000000</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E154" s="5"/>
-      <c r="F154" s="4"/>
-      <c r="G154" s="4"/>
-      <c r="H154" s="4" t="s">
-        <v>94</v>
+      <c r="B154" s="57">
+        <v>254582000</v>
+      </c>
+      <c r="C154" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D154" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E154" s="58"/>
+      <c r="F154" s="54"/>
+      <c r="G154" s="54"/>
+      <c r="H154" s="54" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:8">
       <c r="A155" s="4"/>
       <c r="B155" s="41">
-        <v>1000001</v>
+        <v>72900001</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>95</v>
+        <v>248</v>
       </c>
       <c r="E155" s="5"/>
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4" t="s">
-        <v>95</v>
+        <v>248</v>
       </c>
     </row>
     <row r="156" spans="1:8">
       <c r="A156" s="4"/>
-      <c r="B156" s="41">
-        <v>72900001</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B156" s="41"/>
+      <c r="C156" s="4"/>
       <c r="D156" s="4" t="s">
-        <v>96</v>
+        <v>249</v>
       </c>
       <c r="E156" s="5"/>
       <c r="F156" s="4"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4" t="s">
-        <v>96</v>
+        <v>249</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4118,308 +4119,324 @@
       <c r="B157" s="41"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
       <c r="E157" s="5"/>
       <c r="F157" s="4"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
     </row>
     <row r="158" spans="1:8">
       <c r="A158" s="4"/>
-      <c r="B158" s="41"/>
-      <c r="C158" s="4"/>
+      <c r="B158" s="41">
+        <v>68496003</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D158" s="4" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="E158" s="5"/>
       <c r="F158" s="4"/>
       <c r="G158" s="4"/>
       <c r="H158" s="4" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" s="4"/>
       <c r="B159" s="41">
-        <v>68496003</v>
+        <v>34000006</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="E159" s="5"/>
       <c r="F159" s="4"/>
       <c r="G159" s="4"/>
       <c r="H159" s="4" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" s="4"/>
       <c r="B160" s="41">
-        <v>34000006</v>
+        <v>10743008</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="E160" s="5"/>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="4"/>
       <c r="B161" s="41">
-        <v>10743008</v>
+        <v>64766004</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>101</v>
+        <v>254</v>
       </c>
       <c r="E161" s="5"/>
       <c r="F161" s="4"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4" t="s">
-        <v>101</v>
+        <v>254</v>
       </c>
     </row>
     <row r="162" spans="1:8">
       <c r="A162" s="4"/>
       <c r="B162" s="41">
-        <v>64766004</v>
+        <v>119292006</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="E162" s="5"/>
       <c r="F162" s="4"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="163" spans="1:8">
       <c r="A163" s="4"/>
-      <c r="B163" s="41">
-        <v>119292006</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B163" s="41"/>
+      <c r="C163" s="4"/>
       <c r="D163" s="4" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="E163" s="5"/>
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
       <c r="H163" s="4" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="4"/>
-      <c r="B164" s="41"/>
-      <c r="C164" s="4"/>
+      <c r="B164" s="41">
+        <v>56265001</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D164" s="4" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="E164" s="5"/>
       <c r="F164" s="4"/>
       <c r="G164" s="4"/>
       <c r="H164" s="4" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
     </row>
     <row r="165" spans="1:8">
       <c r="A165" s="4"/>
       <c r="B165" s="41">
-        <v>56265001</v>
+        <v>22298006</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="E165" s="5"/>
       <c r="F165" s="4"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="4"/>
       <c r="B166" s="41">
-        <v>22298006</v>
+        <v>53741008</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="E166" s="5"/>
       <c r="F166" s="4"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
     </row>
     <row r="167" spans="1:8">
       <c r="A167" s="4"/>
       <c r="B167" s="41">
-        <v>53741008</v>
+        <v>194828000</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="E167" s="5"/>
       <c r="F167" s="4"/>
       <c r="G167" s="4"/>
       <c r="H167" s="4" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
     </row>
     <row r="168" spans="1:8">
       <c r="A168" s="4"/>
-      <c r="B168" s="41">
-        <v>194828000</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B168" s="41"/>
+      <c r="C168" s="4"/>
       <c r="D168" s="4" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="E168" s="5"/>
       <c r="F168" s="4"/>
       <c r="G168" s="4"/>
       <c r="H168" s="4" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="169" spans="1:8">
       <c r="A169" s="4"/>
-      <c r="B169" s="41"/>
-      <c r="C169" s="4"/>
+      <c r="B169" s="41">
+        <v>128053003</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="D169" s="4" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="E169" s="5"/>
       <c r="F169" s="4"/>
       <c r="G169" s="4"/>
       <c r="H169" s="4" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
     </row>
     <row r="170" spans="1:8">
       <c r="A170" s="4"/>
       <c r="B170" s="41">
-        <v>128053003</v>
+        <v>59282003</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="E170" s="5"/>
       <c r="F170" s="4"/>
       <c r="G170" s="4"/>
       <c r="H170" s="4" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
     </row>
     <row r="171" spans="1:8">
       <c r="A171" s="4"/>
       <c r="B171" s="41">
-        <v>59282003</v>
+        <v>4779008</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="E171" s="5"/>
       <c r="F171" s="4"/>
       <c r="G171" s="4"/>
       <c r="H171" s="4" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="4"/>
-      <c r="B172" s="41">
-        <v>4779008</v>
-      </c>
-      <c r="C172" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B172" s="41"/>
+      <c r="C172" s="4"/>
       <c r="D172" s="4" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="E172" s="5"/>
       <c r="F172" s="4"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
     </row>
     <row r="173" spans="1:8">
-      <c r="A173" s="4"/>
-      <c r="B173" s="41"/>
-      <c r="C173" s="4"/>
-      <c r="D173" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E173" s="5"/>
-      <c r="F173" s="4"/>
-      <c r="G173" s="4"/>
-      <c r="H173" s="4" t="s">
-        <v>201</v>
+      <c r="A173" s="59"/>
+      <c r="B173" s="57">
+        <v>315645005</v>
+      </c>
+      <c r="C173" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D173" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="E173" s="58"/>
+      <c r="F173" s="54"/>
+      <c r="G173" s="54"/>
+      <c r="H173" s="54" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="174" spans="1:8">
-      <c r="A174" s="4"/>
-      <c r="B174" s="41"/>
-      <c r="C174" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D174" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E174" s="5"/>
-      <c r="F174" s="4"/>
-      <c r="G174" s="4"/>
-      <c r="H174" s="4" t="s">
-        <v>202</v>
-      </c>
+      <c r="A174" s="60"/>
+      <c r="B174" s="53">
+        <v>160245001</v>
+      </c>
+      <c r="C174" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="D174" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E174" s="55"/>
+      <c r="F174" s="52"/>
+      <c r="G174" s="52"/>
+      <c r="H174" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="2:8">
+      <c r="B181" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181" s="52"/>
+      <c r="D181" s="52"/>
+      <c r="E181" s="55"/>
+      <c r="F181" s="52"/>
+      <c r="G181" s="52"/>
+      <c r="H181" s="56"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="12" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>